<commit_message>
ranking only with click y/n
</commit_message>
<xml_diff>
--- a/practica-LOINC/loinc_dataset-v2.xlsx
+++ b/practica-LOINC/loinc_dataset-v2.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="231">
   <si>
     <t xml:space="preserve">Query: GLUCOSE IN BLOOD</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t xml:space="preserve">Urine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
   </si>
   <si>
     <t xml:space="preserve">1798-8</t>
@@ -816,10 +819,10 @@
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.73"/>
   </cols>
@@ -1075,73 +1078,73 @@
       <c r="E16" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="0" t="n">
-        <v>3</v>
+      <c r="F16" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>34</v>
@@ -1149,16 +1152,16 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>22</v>
@@ -1166,10 +1169,10 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>56</v>
@@ -1180,39 +1183,39 @@
       <c r="E22" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="0" t="n">
-        <v>2</v>
+      <c r="F22" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>56</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="0" t="n">
-        <v>4</v>
+      <c r="F23" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>12</v>
@@ -1223,13 +1226,13 @@
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>12</v>
@@ -1240,87 +1243,87 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>56</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="0" t="n">
-        <v>1</v>
+      <c r="F27" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>30</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>13</v>
@@ -1328,30 +1331,30 @@
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>12</v>
@@ -1359,19 +1362,19 @@
       <c r="E32" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="F32" s="0" t="n">
-        <v>4</v>
+      <c r="F32" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>17</v>
@@ -1382,13 +1385,13 @@
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>12</v>
@@ -1399,13 +1402,13 @@
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>12</v>
@@ -1416,13 +1419,13 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>12</v>
@@ -1433,30 +1436,30 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>26</v>
@@ -1467,13 +1470,13 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>17</v>
@@ -1484,30 +1487,30 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>17</v>
@@ -1518,16 +1521,16 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E42" s="0" t="s">
         <v>13</v>
@@ -1535,44 +1538,44 @@
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>46</v>
@@ -1586,13 +1589,13 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>50</v>
@@ -1603,10 +1606,10 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>11</v>
@@ -1620,47 +1623,47 @@
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>30</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>12</v>
@@ -1671,16 +1674,16 @@
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E51" s="0" t="s">
         <v>22</v>
@@ -1688,13 +1691,13 @@
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>26</v>
@@ -1705,13 +1708,13 @@
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>12</v>
@@ -1722,33 +1725,33 @@
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E54" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F54" s="0" t="n">
-        <v>3</v>
+      <c r="F54" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>26</v>
@@ -1759,30 +1762,30 @@
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>12</v>
@@ -1793,13 +1796,13 @@
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>12</v>
@@ -1810,30 +1813,30 @@
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>12</v>
@@ -1844,27 +1847,27 @@
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>37</v>
@@ -1878,30 +1881,30 @@
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>26</v>
@@ -1912,13 +1915,13 @@
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>12</v>
@@ -1929,30 +1932,30 @@
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>26</v>
@@ -1963,13 +1966,13 @@
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>26</v>
@@ -1980,13 +1983,13 @@
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>12</v>
@@ -1997,13 +2000,13 @@
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>26</v>
@@ -2030,18 +2033,18 @@
   </sheetPr>
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="71.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="71.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2072,36 +2075,36 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2157,13 +2160,13 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>26</v>
@@ -2174,16 +2177,16 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>34</v>
@@ -2191,13 +2194,13 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>17</v>
@@ -2208,30 +2211,30 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>12</v>
@@ -2239,33 +2242,33 @@
       <c r="E13" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="0" t="n">
-        <v>2</v>
+      <c r="F13" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>11</v>
@@ -2279,13 +2282,13 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>26</v>
@@ -2296,13 +2299,13 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>17</v>
@@ -2327,19 +2330,19 @@
       <c r="E18" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="0" t="n">
-        <v>1</v>
+      <c r="F18" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>12</v>
@@ -2367,30 +2370,30 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>26</v>
@@ -2401,13 +2404,13 @@
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>26</v>
@@ -2452,16 +2455,16 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>22</v>
@@ -2469,13 +2472,13 @@
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>12</v>
@@ -2486,27 +2489,27 @@
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>37</v>
@@ -2520,13 +2523,13 @@
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>17</v>
@@ -2537,13 +2540,13 @@
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>26</v>
@@ -2554,13 +2557,13 @@
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>12</v>
@@ -2568,39 +2571,39 @@
       <c r="E32" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="0" t="n">
-        <v>3</v>
+      <c r="F32" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>56</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>13</v>
@@ -2608,16 +2611,16 @@
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>56</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>18</v>
@@ -2625,22 +2628,22 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="F36" s="0" t="n">
-        <v>4</v>
+        <v>194</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2662,13 +2665,13 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>12</v>
@@ -2679,30 +2682,30 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>50</v>
@@ -2711,35 +2714,32 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>30</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="F41" s="0" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>26</v>
@@ -2750,30 +2750,30 @@
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>12</v>
@@ -2784,10 +2784,10 @@
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>56</v>
@@ -2801,16 +2801,16 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E46" s="0" t="s">
         <v>22</v>
@@ -2818,30 +2818,30 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>12</v>
@@ -2852,16 +2852,16 @@
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E49" s="0" t="s">
         <v>13</v>
@@ -2869,13 +2869,13 @@
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>12</v>
@@ -2903,13 +2903,13 @@
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>12</v>
@@ -2920,16 +2920,16 @@
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E53" s="0" t="s">
         <v>22</v>
@@ -2937,13 +2937,13 @@
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>26</v>
@@ -2954,13 +2954,13 @@
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>12</v>
@@ -2971,13 +2971,13 @@
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>12</v>
@@ -2988,27 +2988,27 @@
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>46</v>
@@ -3022,53 +3022,53 @@
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3124,47 +3124,47 @@
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>12</v>
@@ -3175,13 +3175,13 @@
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>12</v>
@@ -3192,22 +3192,19 @@
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>30</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="F69" s="0" t="n">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3246,17 +3243,17 @@
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="80.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3287,30 +3284,30 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>12</v>
@@ -3321,16 +3318,16 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>13</v>
@@ -3338,13 +3335,13 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>26</v>
@@ -3355,13 +3352,13 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>26</v>
@@ -3372,10 +3369,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>56</v>
@@ -3389,30 +3386,30 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>26</v>
@@ -3423,30 +3420,30 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>12</v>
@@ -3457,16 +3454,16 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>34</v>
@@ -3491,30 +3488,30 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>12</v>
@@ -3525,53 +3522,50 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="0" t="n">
-        <v>5</v>
-      </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>17</v>
@@ -3582,19 +3576,19 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3633,13 +3627,13 @@
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>26</v>
@@ -3650,16 +3644,16 @@
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>22</v>
@@ -3667,22 +3661,19 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="F26" s="0" t="n">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3704,10 +3695,10 @@
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>46</v>
@@ -3721,13 +3712,13 @@
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>12</v>
@@ -3738,13 +3729,13 @@
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>12</v>
@@ -3770,38 +3761,35 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F32" s="0" t="n">
-        <v>6</v>
-      </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>13</v>
@@ -3809,13 +3797,13 @@
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>12</v>
@@ -3826,33 +3814,33 @@
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>56</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>18</v>
@@ -3877,10 +3865,10 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>37</v>
@@ -3894,13 +3882,13 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>26</v>
@@ -3911,13 +3899,13 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>12</v>
@@ -3962,13 +3950,13 @@
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>12</v>
@@ -3996,13 +3984,13 @@
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>12</v>
@@ -4013,13 +4001,13 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>12</v>
@@ -4047,19 +4035,19 @@
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4081,16 +4069,16 @@
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>56</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E50" s="0" t="s">
         <v>13</v>
@@ -4098,13 +4086,13 @@
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>12</v>
@@ -4115,30 +4103,30 @@
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>26</v>
@@ -4149,13 +4137,13 @@
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>12</v>
@@ -4166,30 +4154,30 @@
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>17</v>
@@ -4200,13 +4188,13 @@
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>12</v>
@@ -4217,30 +4205,30 @@
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>50</v>
@@ -4251,10 +4239,10 @@
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>11</v>
@@ -4285,64 +4273,64 @@
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>17</v>
@@ -4353,36 +4341,36 @@
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4404,30 +4392,30 @@
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>26</v>

</xml_diff>